<commit_message>
adds updated queries, updates metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_recapture_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_recapture_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E14DA4-5499-4216-8FCC-EC5196C146A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7ACB34CD-6DE5-438E-B86C-630B9EB61666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="2390" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -226,9 +226,6 @@
     <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
   </si>
   <si>
-    <t>2024-03-29 10:45:51</t>
-  </si>
-  <si>
     <t>2022-02-02 10:00:10</t>
   </si>
   <si>
@@ -326,11 +323,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,9 +545,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18:D20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1316,11 +1313,11 @@
         <v>34</v>
       </c>
       <c r="K19" s="2"/>
-      <c r="L19" s="14" t="s">
+      <c r="L19" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M19" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="M19" s="14" t="s">
-        <v>66</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
@@ -1360,11 +1357,11 @@
         <v>34</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="14" t="s">
+      <c r="L20" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M20" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="M20" s="14" t="s">
-        <v>68</v>
       </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
@@ -1381,7 +1378,7 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="12"/>
+      <c r="A21" s="13"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
@@ -1409,7 +1406,7 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="13"/>
+      <c r="A22" s="14"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>

</xml_diff>

<commit_message>
adds notes and generates clean data files
</commit_message>
<xml_diff>
--- a/data-raw/metadata/lower_feather_recapture_metadata.xlsx
+++ b/data-raw/metadata/lower_feather_recapture_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-lower-feather-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB31B63D-9ED1-423A-9020-E6EA0FCBF045}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEA5A843-709A-47B7-8FB8-9C79444A8300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1620" yWindow="870" windowWidth="20470" windowHeight="11390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>2024-03-31 08:30:21</t>
+  </si>
+  <si>
+    <t>2024-03-31 10:45:51</t>
   </si>
 </sst>
 </file>
@@ -545,9 +548,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z982"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1317,7 +1320,7 @@
         <v>66</v>
       </c>
       <c r="M19" s="12" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>

</xml_diff>